<commit_message>
Changed to multiple choice
</commit_message>
<xml_diff>
--- a/week2/MyMenu/menu.xlsx
+++ b/week2/MyMenu/menu.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -64,6 +64,12 @@
   </x:si>
   <x:si>
     <x:t>Spicy Cheesy Bread</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Heart Pan Pizza</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lasagna</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -525,6 +531,34 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>10.1</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>69.2</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>